<commit_message>
16th - finish notices, start on dashboard
</commit_message>
<xml_diff>
--- a/BugTracker-classes_v2.xlsx
+++ b/BugTracker-classes_v2.xlsx
@@ -9,16 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="22290" windowHeight="7710"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="22290" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Classes!$A$1:$V$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Classes!$A$1:$V$28</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
     <t>Ticket</t>
   </si>
@@ -144,15 +143,9 @@
     <t>LogId</t>
   </si>
   <si>
-    <t>MediaURL</t>
-  </si>
-  <si>
     <t>Started</t>
   </si>
   <si>
-    <t>RepositoryURL</t>
-  </si>
-  <si>
     <t>ProjectId</t>
   </si>
   <si>
@@ -373,6 +366,48 @@
   </si>
   <si>
     <t>IsArchived</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>(Tkt) Stage</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Step (int)</t>
+  </si>
+  <si>
+    <t>(Pjt) Phase</t>
   </si>
 </sst>
 </file>
@@ -481,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -533,6 +568,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -819,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:V23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,10 +871,10 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.42578125" customWidth="1"/>
     <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="1.42578125" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="1.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -860,15 +896,15 @@
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O1" s="27"/>
       <c r="R1" s="1" t="s">
@@ -908,25 +944,25 @@
       </c>
       <c r="O2" s="27"/>
       <c r="P2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="V2" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -938,7 +974,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s">
@@ -946,7 +982,7 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" t="s">
@@ -954,13 +990,13 @@
       </c>
       <c r="O3" s="27"/>
       <c r="P3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="V3" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -970,11 +1006,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -982,25 +1016,25 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="O4" s="27"/>
       <c r="P4" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="11"/>
       <c r="T4" s="12"/>
       <c r="U4" s="13"/>
       <c r="V4" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1010,7 +1044,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" t="s">
@@ -1018,18 +1052,18 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O5" s="27"/>
       <c r="P5" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R5" s="26"/>
       <c r="S5" s="19"/>
@@ -1038,11 +1072,11 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" t="s">
@@ -1060,10 +1094,10 @@
       </c>
       <c r="O6" s="27"/>
       <c r="P6" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="16"/>
@@ -1077,30 +1111,28 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O7" s="27"/>
       <c r="P7" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R7" s="15"/>
       <c r="S7" s="17"/>
@@ -1112,7 +1144,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" t="s">
@@ -1134,19 +1166,19 @@
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O8" s="27"/>
       <c r="P8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="7"/>
       <c r="V8" s="29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1160,32 +1192,32 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N9" t="s">
         <v>0</v>
       </c>
       <c r="O9" s="27"/>
       <c r="P9" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="T9" s="8"/>
       <c r="U9" s="25"/>
@@ -1195,16 +1227,16 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G10" s="4"/>
       <c r="M10" s="4"/>
       <c r="O10" s="27"/>
       <c r="P10" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="24"/>
@@ -1218,15 +1250,15 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="1" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="1" t="s">
@@ -1234,10 +1266,10 @@
       </c>
       <c r="O11" s="27"/>
       <c r="P11" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="22"/>
@@ -1255,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>3</v>
@@ -1277,10 +1309,10 @@
       </c>
       <c r="O12" s="27"/>
       <c r="P12" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R12" s="15"/>
       <c r="S12" s="23"/>
@@ -1296,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
@@ -1312,17 +1344,17 @@
       </c>
       <c r="O13" s="27"/>
       <c r="P13" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
       <c r="V13" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1334,7 +1366,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
@@ -1350,10 +1382,10 @@
       </c>
       <c r="O14" s="27"/>
       <c r="P14" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R14" s="15"/>
       <c r="S14" s="17"/>
@@ -1363,13 +1395,13 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="2" t="s">
@@ -1385,10 +1417,10 @@
       </c>
       <c r="O15" s="27"/>
       <c r="P15" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="3"/>
@@ -1397,13 +1429,13 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="2" t="s">
@@ -1411,32 +1443,32 @@
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O16" s="27"/>
       <c r="P16" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="2" t="s">
@@ -1452,21 +1484,21 @@
       </c>
       <c r="O17" s="27"/>
       <c r="P17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1481,14 +1513,14 @@
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1499,7 +1531,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1510,52 +1542,55 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M19" s="4"/>
       <c r="O19" s="27"/>
       <c r="P19" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="M20" s="4"/>
       <c r="O20" s="27"/>
       <c r="P20" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="O21" s="27"/>
     </row>
@@ -1564,7 +1599,15 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="1"/>
+      <c r="J22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>19</v>
       </c>
       <c r="O22" s="27"/>
     </row>
@@ -1573,19 +1616,93 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="M23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
+      <c r="K24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="2">
+        <v>6</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="2">
+        <v>7</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M26" s="2">
+        <v>8</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J27" s="2">
+        <v>3</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M27" s="2">
+        <v>9</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
+      <c r="J28" s="2">
+        <v>4</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="M28" s="2">
+        <v>10</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="P16:V20">
-    <sortCondition ref="P16"/>
+  <sortState ref="H26:H28">
+    <sortCondition ref="H25"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="V3" r:id="rId1"/>
@@ -1593,7 +1710,7 @@
     <hyperlink ref="V8" r:id="rId3"/>
     <hyperlink ref="V13" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="79" orientation="landscape" r:id="rId5"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="84" orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>